<commit_message>
Rename key to cd
</commit_message>
<xml_diff>
--- a/app/assets/xlsx/bill.xlsx
+++ b/app/assets/xlsx/bill.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sito/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ishida/Projects/nebill/app/assets/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="37000" yWindow="780" windowWidth="27640" windowHeight="18640"/>
+    <workbookView xWindow="37000" yWindow="-640" windowWidth="27640" windowHeight="18640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="請求書" sheetId="34" r:id="rId1"/>
@@ -273,26 +273,11 @@
     <phoneticPr fontId="16"/>
   </si>
   <si>
-    <t>請求書No.：[bill_key]</t>
-    <rPh sb="0" eb="3">
-      <t>セイキュウショ</t>
-    </rPh>
-    <phoneticPr fontId="16"/>
-  </si>
-  <si>
-    <t>PJNo.：[project_key]</t>
-    <phoneticPr fontId="16"/>
-  </si>
-  <si>
     <t>[project_name]</t>
     <phoneticPr fontId="16"/>
   </si>
   <si>
     <t>[bill_payment_on]</t>
-    <phoneticPr fontId="16"/>
-  </si>
-  <si>
-    <t>PJNo.：[project_key]</t>
     <phoneticPr fontId="16"/>
   </si>
   <si>
@@ -367,6 +352,21 @@
   </si>
   <si>
     <t>[total]</t>
+    <phoneticPr fontId="16"/>
+  </si>
+  <si>
+    <t>PJNo.：[project_cd]</t>
+    <phoneticPr fontId="16"/>
+  </si>
+  <si>
+    <t>請求書No.：[bill_cd]</t>
+    <rPh sb="0" eb="3">
+      <t>セイキュウショ</t>
+    </rPh>
+    <phoneticPr fontId="16"/>
+  </si>
+  <si>
+    <t>PJNo.：[project_cd]</t>
     <phoneticPr fontId="16"/>
   </si>
 </sst>
@@ -1821,8 +1821,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1838,7 +1838,7 @@
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="H1" s="45" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -1876,14 +1876,14 @@
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="59" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="G7" s="59"/>
       <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="60" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="G8" s="60"/>
       <c r="H8" s="44"/>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="63" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" s="63"/>
       <c r="E14" s="63"/>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="64" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D16" s="64"/>
       <c r="E16" s="13"/>
@@ -1957,7 +1957,7 @@
     <row r="19" spans="1:9" s="19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="15"/>
       <c r="B19" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -1965,14 +1965,14 @@
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
       <c r="H19" s="52" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="20"/>
       <c r="B20" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="22"/>
@@ -1992,7 +1992,7 @@
       <c r="F21" s="28"/>
       <c r="G21" s="25"/>
       <c r="H21" s="52" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2139,7 +2139,7 @@
       <c r="F35" s="39"/>
       <c r="G35" s="40"/>
       <c r="H35" s="53" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I35" s="34"/>
     </row>
@@ -2154,7 +2154,7 @@
       <c r="F36" s="39"/>
       <c r="G36" s="40"/>
       <c r="H36" s="56" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I36" s="34"/>
     </row>
@@ -2169,7 +2169,7 @@
       <c r="F37" s="39"/>
       <c r="G37" s="40"/>
       <c r="H37" s="55" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I37" s="34"/>
     </row>
@@ -2184,7 +2184,7 @@
       <c r="F38" s="39"/>
       <c r="G38" s="40"/>
       <c r="H38" s="53" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I38" s="1"/>
     </row>
@@ -2200,7 +2200,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D42" s="58"/>
       <c r="I42" s="1"/>
@@ -2255,8 +2255,8 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2273,7 +2273,7 @@
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="H1" s="45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -2293,7 +2293,7 @@
     <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G4" s="44"/>
       <c r="H4" s="51" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="63" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="63"/>
       <c r="E10" s="63"/>
@@ -2340,7 +2340,7 @@
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="64" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D12" s="64"/>
       <c r="E12" s="13"/>
@@ -2364,7 +2364,7 @@
     <row r="15" spans="1:9" s="19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="15"/>
       <c r="B15" s="16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2372,14 +2372,14 @@
       <c r="F15" s="17"/>
       <c r="G15" s="18"/>
       <c r="H15" s="52" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="20"/>
       <c r="B16" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="22"/>
@@ -2400,7 +2400,7 @@
       <c r="F17" s="28"/>
       <c r="G17" s="25"/>
       <c r="H17" s="52" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2547,7 +2547,7 @@
       <c r="F31" s="39"/>
       <c r="G31" s="40"/>
       <c r="H31" s="53" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I31" s="34"/>
     </row>
@@ -2562,7 +2562,7 @@
       <c r="F32" s="39"/>
       <c r="G32" s="40"/>
       <c r="H32" s="55" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I32" s="34"/>
     </row>
@@ -2577,7 +2577,7 @@
       <c r="F33" s="39"/>
       <c r="G33" s="40"/>
       <c r="H33" s="55" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I33" s="34"/>
     </row>
@@ -2592,7 +2592,7 @@
       <c r="F34" s="39"/>
       <c r="G34" s="40"/>
       <c r="H34" s="53" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I34" s="1"/>
     </row>

</xml_diff>

<commit_message>
[#142744923]Change payment_on to payment_type
</commit_message>
<xml_diff>
--- a/app/assets/xlsx/bill.xlsx
+++ b/app/assets/xlsx/bill.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ishida/Projects/nebill/app/assets/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yamashita/Desktop/nebill/app/assets/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="37000" yWindow="-640" windowWidth="27640" windowHeight="18640" activeTab="1"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="請求書" sheetId="34" r:id="rId1"/>
@@ -277,10 +277,6 @@
     <phoneticPr fontId="16"/>
   </si>
   <si>
-    <t>[bill_payment_on]</t>
-    <phoneticPr fontId="16"/>
-  </si>
-  <si>
     <t>[project_name]</t>
     <phoneticPr fontId="16"/>
   </si>
@@ -367,6 +363,10 @@
   </si>
   <si>
     <t>PJNo.：[project_cd]</t>
+    <phoneticPr fontId="16"/>
+  </si>
+  <si>
+    <t>[bill_payment_type]</t>
     <phoneticPr fontId="16"/>
   </si>
 </sst>
@@ -1414,14 +1414,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1822,7 +1822,7 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:H10"/>
+      <selection activeCell="C42" sqref="C42:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1838,7 +1838,7 @@
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="H1" s="45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -1876,14 +1876,14 @@
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="59"/>
       <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="60"/>
       <c r="H8" s="44"/>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="64" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="64"/>
       <c r="E16" s="13"/>
@@ -1965,14 +1965,14 @@
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
       <c r="H19" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="20"/>
       <c r="B20" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="22"/>
@@ -1992,7 +1992,7 @@
       <c r="F21" s="28"/>
       <c r="G21" s="25"/>
       <c r="H21" s="52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2139,7 +2139,7 @@
       <c r="F35" s="39"/>
       <c r="G35" s="40"/>
       <c r="H35" s="53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I35" s="34"/>
     </row>
@@ -2154,7 +2154,7 @@
       <c r="F36" s="39"/>
       <c r="G36" s="40"/>
       <c r="H36" s="56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I36" s="34"/>
     </row>
@@ -2169,7 +2169,7 @@
       <c r="F37" s="39"/>
       <c r="G37" s="40"/>
       <c r="H37" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I37" s="34"/>
     </row>
@@ -2184,7 +2184,7 @@
       <c r="F38" s="39"/>
       <c r="G38" s="40"/>
       <c r="H38" s="53" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I38" s="1"/>
     </row>
@@ -2200,7 +2200,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D42" s="58"/>
       <c r="I42" s="1"/>
@@ -2273,7 +2273,7 @@
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="H1" s="45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -2293,7 +2293,7 @@
     <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G4" s="44"/>
       <c r="H4" s="51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="63"/>
       <c r="E10" s="63"/>
@@ -2340,7 +2340,7 @@
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="64" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="64"/>
       <c r="E12" s="13"/>
@@ -2364,7 +2364,7 @@
     <row r="15" spans="1:9" s="19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="15"/>
       <c r="B15" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2372,14 +2372,14 @@
       <c r="F15" s="17"/>
       <c r="G15" s="18"/>
       <c r="H15" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="20"/>
       <c r="B16" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="22"/>
@@ -2400,7 +2400,7 @@
       <c r="F17" s="28"/>
       <c r="G17" s="25"/>
       <c r="H17" s="52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2547,7 +2547,7 @@
       <c r="F31" s="39"/>
       <c r="G31" s="40"/>
       <c r="H31" s="53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I31" s="34"/>
     </row>
@@ -2562,7 +2562,7 @@
       <c r="F32" s="39"/>
       <c r="G32" s="40"/>
       <c r="H32" s="55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I32" s="34"/>
     </row>
@@ -2577,7 +2577,7 @@
       <c r="F33" s="39"/>
       <c r="G33" s="40"/>
       <c r="H33" s="55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I33" s="34"/>
     </row>
@@ -2592,7 +2592,7 @@
       <c r="F34" s="39"/>
       <c r="G34" s="40"/>
       <c r="H34" s="53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I34" s="1"/>
     </row>

</xml_diff>

<commit_message>
Implement PDF download function
</commit_message>
<xml_diff>
--- a/app/assets/xlsx/bill.xlsx
+++ b/app/assets/xlsx/bill.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yamashita/Desktop/nebill/app/assets/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sito/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16480" activeTab="1"/>
+    <workbookView xWindow="40160" yWindow="-960" windowWidth="27640" windowHeight="16480"/>
   </bookViews>
   <sheets>
     <sheet name="請求書" sheetId="34" r:id="rId1"/>
@@ -256,16 +256,6 @@
     <t>下記項目の検収が完了致しました。</t>
   </si>
   <si>
-    <t>株式会社御中</t>
-    <rPh sb="0" eb="4">
-      <t>カブシキガイシャ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>オンチュウ</t>
-    </rPh>
-    <phoneticPr fontId="16"/>
-  </si>
-  <si>
     <t>　　超過分：基準H　実働：H　※0.5単位　@/H</t>
     <rPh sb="2" eb="4">
       <t>チョウカ</t>
@@ -367,6 +357,13 @@
   </si>
   <si>
     <t>[bill_payment_type]</t>
+    <phoneticPr fontId="16"/>
+  </si>
+  <si>
+    <t>[bill_company_name]御中</t>
+    <rPh sb="19" eb="21">
+      <t>オンチュウ</t>
+    </rPh>
     <phoneticPr fontId="16"/>
   </si>
 </sst>
@@ -1414,14 +1411,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1821,8 +1818,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42:D42"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1838,13 +1835,13 @@
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="H1" s="45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="61" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -1876,14 +1873,14 @@
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="59"/>
       <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="60"/>
       <c r="H8" s="44"/>
@@ -1917,7 +1914,7 @@
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="63"/>
       <c r="E14" s="63"/>
@@ -1933,7 +1930,7 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="64" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="64"/>
       <c r="E16" s="13"/>
@@ -1957,7 +1954,7 @@
     <row r="19" spans="1:9" s="19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="15"/>
       <c r="B19" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -1965,14 +1962,14 @@
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
       <c r="H19" s="52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="20"/>
       <c r="B20" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="22"/>
@@ -1984,7 +1981,7 @@
     <row r="21" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="20"/>
       <c r="B21" s="43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="22"/>
@@ -1992,7 +1989,7 @@
       <c r="F21" s="28"/>
       <c r="G21" s="25"/>
       <c r="H21" s="52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2139,7 +2136,7 @@
       <c r="F35" s="39"/>
       <c r="G35" s="40"/>
       <c r="H35" s="53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I35" s="34"/>
     </row>
@@ -2154,7 +2151,7 @@
       <c r="F36" s="39"/>
       <c r="G36" s="40"/>
       <c r="H36" s="56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I36" s="34"/>
     </row>
@@ -2169,7 +2166,7 @@
       <c r="F37" s="39"/>
       <c r="G37" s="40"/>
       <c r="H37" s="55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I37" s="34"/>
     </row>
@@ -2184,7 +2181,7 @@
       <c r="F38" s="39"/>
       <c r="G38" s="40"/>
       <c r="H38" s="53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I38" s="1"/>
     </row>
@@ -2200,7 +2197,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" s="58"/>
       <c r="I42" s="1"/>
@@ -2255,7 +2252,7 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -2273,7 +2270,7 @@
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="H1" s="45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -2293,7 +2290,7 @@
     <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G4" s="44"/>
       <c r="H4" s="51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2324,7 +2321,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="63" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="63"/>
       <c r="E10" s="63"/>
@@ -2340,7 +2337,7 @@
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="64" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="64"/>
       <c r="E12" s="13"/>
@@ -2364,7 +2361,7 @@
     <row r="15" spans="1:9" s="19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="15"/>
       <c r="B15" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2372,14 +2369,14 @@
       <c r="F15" s="17"/>
       <c r="G15" s="18"/>
       <c r="H15" s="52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="20"/>
       <c r="B16" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="22"/>
@@ -2400,7 +2397,7 @@
       <c r="F17" s="28"/>
       <c r="G17" s="25"/>
       <c r="H17" s="52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2547,7 +2544,7 @@
       <c r="F31" s="39"/>
       <c r="G31" s="40"/>
       <c r="H31" s="53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I31" s="34"/>
     </row>
@@ -2562,7 +2559,7 @@
       <c r="F32" s="39"/>
       <c r="G32" s="40"/>
       <c r="H32" s="55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I32" s="34"/>
     </row>
@@ -2577,7 +2574,7 @@
       <c r="F33" s="39"/>
       <c r="G33" s="40"/>
       <c r="H33" s="55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I33" s="34"/>
     </row>
@@ -2592,7 +2589,7 @@
       <c r="F34" s="39"/>
       <c r="G34" s="40"/>
       <c r="H34" s="53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I34" s="1"/>
     </row>

</xml_diff>